<commit_message>
Added detailed metrics for portfolio holdings
</commit_message>
<xml_diff>
--- a/Eli Lilly DCF 10-26-22.xlsx
+++ b/Eli Lilly DCF 10-26-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79141B66-03D2-2C40-B83A-A7BD9BDC6089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A83346A-1247-3745-9FA5-805087964272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23680" yWindow="460" windowWidth="27040" windowHeight="26980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25360" windowHeight="26980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1084,10 +1084,10 @@
   <dimension ref="A1:AS112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A104" sqref="A104"/>
+      <selection pane="bottomRight" activeCell="AN96" sqref="AN96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1219,10 +1219,10 @@
         <v>2021</v>
       </c>
       <c r="AM1" s="23">
+        <v>2022</v>
+      </c>
+      <c r="AN1" s="23">
         <v>2023</v>
-      </c>
-      <c r="AN1" s="23">
-        <v>2024</v>
       </c>
       <c r="AO1" s="24" t="s">
         <v>98</v>

</xml_diff>